<commit_message>
GD - Justificación de anulación
</commit_message>
<xml_diff>
--- a/App.Web/App_Data/GDGenerico.xlsx
+++ b/App.Web/App_Data/GDGenerico.xlsx
@@ -5,20 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\source\repos\GestionProcesosV2\App.Web\App_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsilva\source\repos\GestionProcesos\App.Web\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FF6967-FC7D-4464-98E6-29C2F788AE4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A910F4E-7A5A-4783-9EF4-6A619432648B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="-120" windowWidth="23295" windowHeight="13740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="2" r:id="rId1"/>
     <sheet name="Detalle" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Detalle!$A$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Resumen!$A$1:$Q$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Detalle!$A$1:$K$667</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Resumen!$A$1:$S$157</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -30,20 +30,53 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+  <si>
+    <t>Proceso Id</t>
+  </si>
+  <si>
+    <t>Proceso</t>
+  </si>
+  <si>
+    <t>Autor</t>
+  </si>
+  <si>
+    <t>Unidad</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
   <si>
     <t>Materia</t>
   </si>
   <si>
+    <t>Observación</t>
+  </si>
+  <si>
+    <t>Número externo</t>
+  </si>
+  <si>
+    <t>Origen</t>
+  </si>
+  <si>
+    <t>Usuario destino</t>
+  </si>
+  <si>
+    <t>Unidad destino</t>
+  </si>
+  <si>
     <t>Reservado</t>
   </si>
   <si>
+    <t>Referencia</t>
+  </si>
+  <si>
+    <t>Workflow Id</t>
+  </si>
+  <si>
     <t>Tarea</t>
   </si>
   <si>
-    <t>Proceso</t>
-  </si>
-  <si>
     <t>Inicio</t>
   </si>
   <si>
@@ -53,43 +86,16 @@
     <t>Usuario</t>
   </si>
   <si>
-    <t>Unidad</t>
-  </si>
-  <si>
-    <t>Observación</t>
-  </si>
-  <si>
-    <t>Autor</t>
-  </si>
-  <si>
-    <t>Estado</t>
-  </si>
-  <si>
-    <t>Creación</t>
-  </si>
-  <si>
-    <t>Fecha ingreso</t>
-  </si>
-  <si>
-    <t>referencia</t>
-  </si>
-  <si>
-    <t>Número externo</t>
-  </si>
-  <si>
-    <t>Origen</t>
-  </si>
-  <si>
-    <t>Usuario destino</t>
-  </si>
-  <si>
-    <t>Unidad destino</t>
-  </si>
-  <si>
-    <t>Workflow Id</t>
-  </si>
-  <si>
-    <t>Proceso Id</t>
+    <t>Inicio proceso</t>
+  </si>
+  <si>
+    <t>Fecha ingreso GD</t>
+  </si>
+  <si>
+    <t>Fecha creación GD</t>
+  </si>
+  <si>
+    <t>Término proceso</t>
   </si>
 </sst>
 </file>
@@ -418,7 +424,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -431,59 +437,69 @@
     <col min="3" max="3" width="24" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" style="3" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" style="3"/>
+    <col min="6" max="6" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" style="3" customWidth="1"/>
+    <col min="17" max="17" width="18.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="P1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:S157" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
@@ -512,38 +528,38 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K1" xr:uid="{4BB693B7-A6B0-4D5A-BE50-2E2472504F11}"/>
+  <autoFilter ref="A1:K667" xr:uid="{4BB693B7-A6B0-4D5A-BE50-2E2472504F11}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>